<commit_message>
Se crea el primer prototipo por terminal funcional
</commit_message>
<xml_diff>
--- a/consumibles.xlsx
+++ b/consumibles.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,6 +491,26 @@
         <v>15</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1pmk193ci/a</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Rack A</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Se crea el primer ejecutable del prototipo
</commit_message>
<xml_diff>
--- a/consumibles.xlsx
+++ b/consumibles.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,6 +511,26 @@
         <v>10</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Testeo</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>444555</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Rack A</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>